<commit_message>
Updates for AEMO validation work
</commit_message>
<xml_diff>
--- a/tests/validation_results/Validation_Inputs.xlsx
+++ b/tests/validation_results/Validation_Inputs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA85364-81D6-4687-AB28-18A6B7D620C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D3DB151-3358-4158-AEA3-CDC4E235ACC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32550" yWindow="1875" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2535" yWindow="2385" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -4083,7 +4083,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:AB166"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:G7"/>
     </sheetView>
   </sheetViews>
@@ -12798,7 +12798,7 @@
       <c r="S166" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <autoFilter ref="A5:S166" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="12">
     <mergeCell ref="A1:B1"/>
@@ -12877,7 +12877,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:D10"/>
     </sheetView>
   </sheetViews>
@@ -13568,7 +13568,7 @@
       <c r="D103" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <autoFilter ref="A4:D103" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:A8">
     <sortCondition ref="A5:A8"/>
@@ -14612,6 +14612,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -14763,27 +14783,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14799,28 +14823,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated to validate working successfully with PF 2020
</commit_message>
<xml_diff>
--- a/tests/validation_results/Validation_Inputs.xlsx
+++ b/tests/validation_results/Validation_Inputs.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A925B23-32E0-43BF-B540-3E805940E1B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{569D0D12-0C93-4552-BA5E-571E3F3E8E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2760" windowWidth="21600" windowHeight="11385" tabRatio="868" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -1728,9 +1728,6 @@
     <t>C:\Users\david\PycharmProjects\JA7896-AEMO_PF_Harmonic_Tool\tests\validation_results</t>
   </si>
   <si>
-    <t>AEMO_VIC_V0_20200723</t>
-  </si>
-  <si>
     <t>Medium Load Case</t>
   </si>
   <si>
@@ -1831,6 +1828,9 @@
   </si>
   <si>
     <t>Include_Loci</t>
+  </si>
+  <si>
+    <t>AEMO_VIC_V0_TEST_CASE</t>
   </si>
 </sst>
 </file>
@@ -3713,8 +3713,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3843,7 +3843,7 @@
     </row>
     <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B13" s="30" t="b">
         <v>1</v>
@@ -3887,7 +3887,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -3935,44 +3935,44 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>181</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="22" t="s">
         <v>221</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>222</v>
-      </c>
       <c r="D6" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>221</v>
+        <v>255</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4066,7 +4066,7 @@
       <c r="D22" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="A2:D3"/>
@@ -4317,13 +4317,13 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>189</v>
@@ -4355,22 +4355,22 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>189</v>
       </c>
       <c r="E7" s="18" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>235</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>236</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>189</v>
@@ -9350,55 +9350,55 @@
         <v>0</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="F5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="H5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="J5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="K5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="L5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="N5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="O5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="P5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q5" s="53" t="s">
         <v>165</v>
       </c>
       <c r="R5" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="S5" s="53" t="s">
         <v>165</v>
@@ -9406,10 +9406,10 @@
     </row>
     <row r="6" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>214</v>
@@ -9433,10 +9433,10 @@
     </row>
     <row r="7" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>214</v>
@@ -12927,13 +12927,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D5" s="18" t="b">
         <v>0</v>
@@ -12941,13 +12941,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D6" s="18" t="b">
         <v>0</v>
@@ -12955,13 +12955,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D7" s="18" t="b">
         <v>0</v>
@@ -12969,13 +12969,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D8" s="18" t="b">
         <v>0</v>
@@ -12983,13 +12983,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D9" s="18" t="b">
         <v>0</v>
@@ -12997,13 +12997,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B10" s="18" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>251</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>252</v>
       </c>
       <c r="D10" s="18" t="b">
         <v>0</v>
@@ -13619,7 +13619,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
@@ -14612,6 +14612,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </iab7cdb7554d4997ae876b11632fa575>
+    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9B3B8AC64AC88418540180D602CE6AB" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c03373d3e8f67dac2598d545e73c3e0f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3cada6dc-2705-46ed-bab2-0b2cd6d935ca" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f693bfc3a603cfa0c3f0b58e702f3d19" ns2:_="">
     <xsd:import namespace="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
@@ -14763,27 +14783,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </iab7cdb7554d4997ae876b11632fa575>
-    <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A5E1C23-6545-45A2-BF0C-826678B16173}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14799,28 +14823,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>